<commit_message>
<localdec> removed from <statements>
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlou\Documents\CompilerDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4546FED8-2731-4CC1-8CC9-941C2C064548}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62154DB4-9790-4B25-823C-88AECCFD3C37}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
     <workbookView xWindow="-30" yWindow="7050" windowWidth="14400" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF02000000}"/>
@@ -21,7 +21,7 @@
     <sheet name="PREDICT TABLE" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">CFG!$A$1:$D$250</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">CFG!$A$1:$D$249</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'FOLLOW SET'!$A$1:$D$100</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3387" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3353" uniqueCount="895">
   <si>
     <t>#</t>
   </si>
@@ -2724,6 +2724,15 @@
   </si>
   <si>
     <t>BOOL_LIT &lt;next1dboolarrval&gt;</t>
+  </si>
+  <si>
+    <t>PRELUDE &lt;global&gt; CONCERT(){ &lt;localdec&gt; &lt;statements&gt; } ENCORE</t>
+  </si>
+  <si>
+    <t>INTERLUDE &lt;datatype&gt; id(&lt;funcparam&gt;){ &lt;localdec&gt; &lt;statements&gt; PRODUCE &lt;returnval&gt; }</t>
+  </si>
+  <si>
+    <t>INTERLUDE MUTE id(&lt;funcparam&gt;){ &lt;localdec&gt; &lt;statements&gt; }</t>
   </si>
 </sst>
 </file>
@@ -3648,13 +3657,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G278"/>
+  <dimension ref="A1:G277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="1">
-      <selection activeCell="D132" sqref="D132"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3703,7 +3712,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>96</v>
+        <v>892</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4867,15 +4876,7 @@
       <c r="D86" s="4" t="s">
         <v>855</v>
       </c>
-      <c r="E86" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="F86" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G86" s="4" t="s">
-        <v>856</v>
-      </c>
+      <c r="F86" s="52"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
@@ -4890,15 +4891,9 @@
       <c r="D87" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E87" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="F87" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G87" s="53" t="s">
-        <v>6</v>
-      </c>
+      <c r="E87" s="52"/>
+      <c r="F87" s="52"/>
+      <c r="G87" s="53"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
@@ -4913,15 +4908,7 @@
       <c r="D88" s="4" t="s">
         <v>847</v>
       </c>
-      <c r="E88" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="F88" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G88" s="4" t="s">
-        <v>857</v>
-      </c>
+      <c r="F88" s="52"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
@@ -4936,15 +4923,7 @@
       <c r="D89" s="4" t="s">
         <v>848</v>
       </c>
-      <c r="E89" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="F89" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G89" s="4" t="s">
-        <v>858</v>
-      </c>
+      <c r="F89" s="52"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
@@ -4959,15 +4938,7 @@
       <c r="D90" s="4" t="s">
         <v>849</v>
       </c>
-      <c r="E90" s="55" t="s">
-        <v>857</v>
-      </c>
-      <c r="F90" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G90" s="4" t="s">
-        <v>864</v>
-      </c>
+      <c r="F90" s="52"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
@@ -4982,15 +4953,7 @@
       <c r="D91" s="4" t="s">
         <v>851</v>
       </c>
-      <c r="E91" s="55" t="s">
-        <v>859</v>
-      </c>
-      <c r="F91" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G91" s="4" t="s">
-        <v>860</v>
-      </c>
+      <c r="F91" s="52"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
@@ -5005,15 +4968,8 @@
       <c r="D92" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E92" s="55" t="s">
-        <v>859</v>
-      </c>
-      <c r="F92" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G92" s="53" t="s">
-        <v>6</v>
-      </c>
+      <c r="F92" s="52"/>
+      <c r="G92" s="53"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
@@ -5028,15 +4984,7 @@
       <c r="D93" s="4" t="s">
         <v>852</v>
       </c>
-      <c r="E93" s="55" t="s">
-        <v>858</v>
-      </c>
-      <c r="F93" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="4" t="s">
-        <v>861</v>
-      </c>
+      <c r="F93" s="52"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
@@ -5051,15 +4999,7 @@
       <c r="D94" s="4" t="s">
         <v>854</v>
       </c>
-      <c r="E94" s="55" t="s">
-        <v>862</v>
-      </c>
-      <c r="F94" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G94" s="4" t="s">
-        <v>863</v>
-      </c>
+      <c r="F94" s="52"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
@@ -5074,15 +5014,8 @@
       <c r="D95" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E95" s="55" t="s">
-        <v>862</v>
-      </c>
-      <c r="F95" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G95" s="53" t="s">
-        <v>6</v>
-      </c>
+      <c r="F95" s="52"/>
+      <c r="G95" s="53"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
@@ -5097,9 +5030,7 @@
       <c r="D96" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="F96" s="52" t="s">
-        <v>9</v>
-      </c>
+      <c r="F96" s="52"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
@@ -5658,7 +5589,7 @@
         <v>9</v>
       </c>
       <c r="D136" s="53" t="s">
-        <v>714</v>
+        <v>893</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -5672,7 +5603,7 @@
         <v>9</v>
       </c>
       <c r="D137" s="53" t="s">
-        <v>715</v>
+        <v>894</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -5826,7 +5757,7 @@
         <v>9</v>
       </c>
       <c r="D148" s="53" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -5840,7 +5771,7 @@
         <v>9</v>
       </c>
       <c r="D149" s="53" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5854,7 +5785,7 @@
         <v>9</v>
       </c>
       <c r="D150" s="53" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5868,7 +5799,7 @@
         <v>9</v>
       </c>
       <c r="D151" s="53" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5882,7 +5813,7 @@
         <v>9</v>
       </c>
       <c r="D152" s="53" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -5896,7 +5827,7 @@
         <v>9</v>
       </c>
       <c r="D153" s="53" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -5910,7 +5841,7 @@
         <v>9</v>
       </c>
       <c r="D154" s="53" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5918,13 +5849,13 @@
         <v>153</v>
       </c>
       <c r="B155" s="52" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C155" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D155" s="53" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5938,7 +5869,7 @@
         <v>9</v>
       </c>
       <c r="D156" s="53" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5952,7 +5883,7 @@
         <v>9</v>
       </c>
       <c r="D157" s="53" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -5960,13 +5891,13 @@
         <v>156</v>
       </c>
       <c r="B158" s="52" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C158" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D158" s="53" t="s">
-        <v>6</v>
+        <v>740</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -5980,7 +5911,7 @@
         <v>9</v>
       </c>
       <c r="D159" s="53" t="s">
-        <v>740</v>
+        <v>6</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -5988,13 +5919,13 @@
         <v>158</v>
       </c>
       <c r="B160" s="52" t="s">
-        <v>106</v>
+        <v>738</v>
       </c>
       <c r="C160" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D160" s="53" t="s">
-        <v>6</v>
+        <v>739</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -6008,7 +5939,7 @@
         <v>9</v>
       </c>
       <c r="D161" s="53" t="s">
-        <v>739</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -6016,13 +5947,13 @@
         <v>160</v>
       </c>
       <c r="B162" s="52" t="s">
-        <v>738</v>
+        <v>108</v>
       </c>
       <c r="C162" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D162" s="53" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -6036,7 +5967,7 @@
         <v>9</v>
       </c>
       <c r="D163" s="53" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -6050,7 +5981,7 @@
         <v>9</v>
       </c>
       <c r="D164" s="53" t="s">
-        <v>113</v>
+        <v>321</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -6058,13 +5989,13 @@
         <v>163</v>
       </c>
       <c r="B165" s="52" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C165" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D165" s="53" t="s">
-        <v>321</v>
+        <v>13</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -6078,7 +6009,7 @@
         <v>9</v>
       </c>
       <c r="D166" s="53" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -6092,7 +6023,7 @@
         <v>9</v>
       </c>
       <c r="D167" s="53" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -6106,7 +6037,7 @@
         <v>9</v>
       </c>
       <c r="D168" s="53" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -6120,7 +6051,7 @@
         <v>9</v>
       </c>
       <c r="D169" s="53" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -6128,13 +6059,13 @@
         <v>168</v>
       </c>
       <c r="B170" s="52" t="s">
-        <v>116</v>
+        <v>425</v>
       </c>
       <c r="C170" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D170" s="53" t="s">
-        <v>26</v>
+        <v>741</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -6148,7 +6079,7 @@
         <v>9</v>
       </c>
       <c r="D171" s="53" t="s">
-        <v>741</v>
+        <v>6</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -6156,13 +6087,13 @@
         <v>170</v>
       </c>
       <c r="B172" s="52" t="s">
-        <v>425</v>
+        <v>115</v>
       </c>
       <c r="C172" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D172" s="53" t="s">
-        <v>6</v>
+        <v>321</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -6176,7 +6107,7 @@
         <v>9</v>
       </c>
       <c r="D173" s="53" t="s">
-        <v>321</v>
+        <v>116</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -6190,7 +6121,7 @@
         <v>9</v>
       </c>
       <c r="D174" s="53" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -6204,7 +6135,7 @@
         <v>9</v>
       </c>
       <c r="D175" s="53" t="s">
-        <v>113</v>
+        <v>6</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -6212,13 +6143,13 @@
         <v>174</v>
       </c>
       <c r="B176" s="52" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C176" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D176" s="53" t="s">
-        <v>6</v>
+        <v>742</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -6232,21 +6163,21 @@
         <v>9</v>
       </c>
       <c r="D177" s="53" t="s">
-        <v>742</v>
+        <v>6</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="7">
         <v>176</v>
       </c>
-      <c r="B178" s="52" t="s">
-        <v>122</v>
+      <c r="B178" s="55" t="s">
+        <v>123</v>
       </c>
       <c r="C178" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D178" s="53" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -6260,7 +6191,7 @@
         <v>9</v>
       </c>
       <c r="D179" s="53" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -6274,7 +6205,7 @@
         <v>9</v>
       </c>
       <c r="D180" s="53" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -6288,7 +6219,7 @@
         <v>9</v>
       </c>
       <c r="D181" s="53" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -6302,7 +6233,7 @@
         <v>9</v>
       </c>
       <c r="D182" s="53" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -6310,13 +6241,13 @@
         <v>181</v>
       </c>
       <c r="B183" s="55" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C183" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D183" s="53" t="s">
-        <v>6</v>
+        <v>322</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -6324,13 +6255,13 @@
         <v>182</v>
       </c>
       <c r="B184" s="55" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C184" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D184" s="53" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -6338,13 +6269,13 @@
         <v>183</v>
       </c>
       <c r="B185" s="55" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C185" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D185" s="53" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -6352,41 +6283,41 @@
         <v>184</v>
       </c>
       <c r="B186" s="55" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C186" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D186" s="53" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="7">
         <v>185</v>
       </c>
-      <c r="B187" s="55" t="s">
-        <v>127</v>
+      <c r="B187" s="52" t="s">
+        <v>132</v>
       </c>
       <c r="C187" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D187" s="53" t="s">
-        <v>325</v>
+        <v>133</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="7">
         <v>186</v>
       </c>
-      <c r="B188" s="52" t="s">
+      <c r="B188" s="55" t="s">
         <v>132</v>
       </c>
       <c r="C188" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D188" s="53" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -6400,119 +6331,119 @@
         <v>9</v>
       </c>
       <c r="D189" s="53" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A190" s="7">
         <v>188</v>
       </c>
-      <c r="B190" s="55" t="s">
-        <v>132</v>
+      <c r="B190" s="52" t="s">
+        <v>133</v>
       </c>
       <c r="C190" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D190" s="53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="7">
         <v>189</v>
       </c>
-      <c r="B191" s="52" t="s">
-        <v>133</v>
+      <c r="B191" s="55" t="s">
+        <v>135</v>
       </c>
       <c r="C191" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D191" s="53" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="7">
         <v>190</v>
       </c>
-      <c r="B192" s="55" t="s">
+      <c r="B192" s="52" t="s">
         <v>135</v>
       </c>
       <c r="C192" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D192" s="53" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A193" s="7">
         <v>191</v>
       </c>
       <c r="B193" s="52" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C193" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D193" s="53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="7">
         <v>192</v>
       </c>
-      <c r="B194" s="52" t="s">
+      <c r="B194" s="55" t="s">
         <v>136</v>
       </c>
       <c r="C194" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D194" s="53" t="s">
-        <v>830</v>
+        <v>6</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="7">
         <v>193</v>
       </c>
-      <c r="B195" s="55" t="s">
-        <v>136</v>
+      <c r="B195" s="52" t="s">
+        <v>134</v>
       </c>
       <c r="C195" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D195" s="53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A196" s="7">
         <v>194</v>
       </c>
-      <c r="B196" s="52" t="s">
-        <v>134</v>
+      <c r="B196" s="55" t="s">
+        <v>137</v>
       </c>
       <c r="C196" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D196" s="53" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="7">
         <v>195</v>
       </c>
       <c r="B197" s="55" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C197" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D197" s="53" t="s">
-        <v>149</v>
+        <v>13</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6526,21 +6457,21 @@
         <v>9</v>
       </c>
       <c r="D198" s="53" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="7">
         <v>197</v>
       </c>
-      <c r="B199" s="55" t="s">
-        <v>147</v>
+      <c r="B199" s="52" t="s">
+        <v>138</v>
       </c>
       <c r="C199" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D199" s="53" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -6554,7 +6485,7 @@
         <v>9</v>
       </c>
       <c r="D200" s="53" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -6568,21 +6499,21 @@
         <v>9</v>
       </c>
       <c r="D201" s="53" t="s">
-        <v>140</v>
+        <v>6</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="7">
         <v>200</v>
       </c>
-      <c r="B202" s="52" t="s">
-        <v>138</v>
+      <c r="B202" s="55" t="s">
+        <v>141</v>
       </c>
       <c r="C202" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D202" s="53" t="s">
-        <v>6</v>
+        <v>142</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -6590,13 +6521,13 @@
         <v>201</v>
       </c>
       <c r="B203" s="55" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C203" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D203" s="53" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -6604,13 +6535,13 @@
         <v>202</v>
       </c>
       <c r="B204" s="55" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C204" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D204" s="53" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -6624,7 +6555,7 @@
         <v>9</v>
       </c>
       <c r="D205" s="53" t="s">
-        <v>137</v>
+        <v>6</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -6632,13 +6563,13 @@
         <v>204</v>
       </c>
       <c r="B206" s="55" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C206" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D206" s="53" t="s">
-        <v>6</v>
+        <v>148</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -6652,7 +6583,7 @@
         <v>9</v>
       </c>
       <c r="D207" s="53" t="s">
-        <v>148</v>
+        <v>6</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -6660,13 +6591,13 @@
         <v>206</v>
       </c>
       <c r="B208" s="55" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C208" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D208" s="53" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -6680,7 +6611,7 @@
         <v>9</v>
       </c>
       <c r="D209" s="53" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -6694,7 +6625,7 @@
         <v>9</v>
       </c>
       <c r="D210" s="53" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -6708,35 +6639,35 @@
         <v>9</v>
       </c>
       <c r="D211" s="53" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A212" s="7">
         <v>210</v>
       </c>
-      <c r="B212" s="55" t="s">
-        <v>150</v>
+      <c r="B212" s="52" t="s">
+        <v>151</v>
       </c>
       <c r="C212" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D212" s="53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="7">
         <v>211</v>
       </c>
       <c r="B213" s="52" t="s">
-        <v>151</v>
+        <v>341</v>
       </c>
       <c r="C213" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D213" s="53" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -6750,21 +6681,21 @@
         <v>9</v>
       </c>
       <c r="D214" s="53" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A215" s="7">
         <v>213</v>
       </c>
       <c r="B215" s="52" t="s">
-        <v>341</v>
+        <v>152</v>
       </c>
       <c r="C215" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D215" s="53" t="s">
-        <v>13</v>
+        <v>154</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -6772,27 +6703,27 @@
         <v>214</v>
       </c>
       <c r="B216" s="52" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C216" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D216" s="53" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="7">
         <v>215</v>
       </c>
       <c r="B217" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C217" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D217" s="53" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -6806,7 +6737,7 @@
         <v>9</v>
       </c>
       <c r="D218" s="53" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -6820,7 +6751,7 @@
         <v>9</v>
       </c>
       <c r="D219" s="53" t="s">
-        <v>158</v>
+        <v>6</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -6828,13 +6759,13 @@
         <v>218</v>
       </c>
       <c r="B220" s="52" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C220" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D220" s="53" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -6842,13 +6773,13 @@
         <v>219</v>
       </c>
       <c r="B221" s="52" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C221" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D221" s="53" t="s">
-        <v>159</v>
+        <v>24</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -6862,7 +6793,7 @@
         <v>9</v>
       </c>
       <c r="D222" s="53" t="s">
-        <v>24</v>
+        <v>321</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -6876,7 +6807,7 @@
         <v>9</v>
       </c>
       <c r="D223" s="53" t="s">
-        <v>321</v>
+        <v>113</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -6884,13 +6815,13 @@
         <v>222</v>
       </c>
       <c r="B224" s="52" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C224" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D224" s="53" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -6904,7 +6835,7 @@
         <v>9</v>
       </c>
       <c r="D225" s="53" t="s">
-        <v>162</v>
+        <v>6</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -6912,13 +6843,13 @@
         <v>224</v>
       </c>
       <c r="B226" s="52" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C226" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D226" s="53" t="s">
-        <v>6</v>
+        <v>326</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -6926,13 +6857,13 @@
         <v>225</v>
       </c>
       <c r="B227" s="52" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C227" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D227" s="53" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -6946,7 +6877,7 @@
         <v>9</v>
       </c>
       <c r="D228" s="53" t="s">
-        <v>327</v>
+        <v>6</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -6954,13 +6885,13 @@
         <v>227</v>
       </c>
       <c r="B229" s="52" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C229" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D229" s="53" t="s">
-        <v>6</v>
+        <v>164</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -6974,7 +6905,7 @@
         <v>9</v>
       </c>
       <c r="D230" s="53" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -6988,7 +6919,7 @@
         <v>9</v>
       </c>
       <c r="D231" s="53" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -7002,7 +6933,7 @@
         <v>9</v>
       </c>
       <c r="D232" s="53" t="s">
-        <v>166</v>
+        <v>13</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -7016,7 +6947,7 @@
         <v>9</v>
       </c>
       <c r="D233" s="53" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -7030,7 +6961,7 @@
         <v>9</v>
       </c>
       <c r="D234" s="53" t="s">
-        <v>15</v>
+        <v>321</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -7038,13 +6969,13 @@
         <v>233</v>
       </c>
       <c r="B235" s="52" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="C235" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D235" s="53" t="s">
-        <v>321</v>
+        <v>168</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -7058,7 +6989,7 @@
         <v>9</v>
       </c>
       <c r="D236" s="53" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -7072,7 +7003,7 @@
         <v>9</v>
       </c>
       <c r="D237" s="53" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -7086,7 +7017,7 @@
         <v>9</v>
       </c>
       <c r="D238" s="53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -7100,7 +7031,7 @@
         <v>9</v>
       </c>
       <c r="D239" s="53" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -7108,13 +7039,13 @@
         <v>238</v>
       </c>
       <c r="B240" s="52" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C240" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D240" s="53" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -7128,7 +7059,7 @@
         <v>9</v>
       </c>
       <c r="D241" s="53" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -7142,7 +7073,7 @@
         <v>9</v>
       </c>
       <c r="D242" s="53" t="s">
-        <v>175</v>
+        <v>113</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -7156,7 +7087,7 @@
         <v>9</v>
       </c>
       <c r="D243" s="53" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7170,7 +7101,7 @@
         <v>9</v>
       </c>
       <c r="D244" s="53" t="s">
-        <v>116</v>
+        <v>321</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -7178,13 +7109,13 @@
         <v>243</v>
       </c>
       <c r="B245" s="52" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C245" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D245" s="53" t="s">
-        <v>321</v>
+        <v>177</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -7198,21 +7129,21 @@
         <v>9</v>
       </c>
       <c r="D246" s="53" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="7">
         <v>245</v>
       </c>
-      <c r="B247" s="52" t="s">
-        <v>176</v>
+      <c r="B247" s="55" t="s">
+        <v>177</v>
       </c>
       <c r="C247" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D247" s="53" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -7226,7 +7157,7 @@
         <v>9</v>
       </c>
       <c r="D248" s="53" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -7240,7 +7171,7 @@
         <v>9</v>
       </c>
       <c r="D249" s="53" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -7254,7 +7185,7 @@
         <v>9</v>
       </c>
       <c r="D250" s="53" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -7268,7 +7199,7 @@
         <v>9</v>
       </c>
       <c r="D251" s="53" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -7282,35 +7213,35 @@
         <v>9</v>
       </c>
       <c r="D252" s="53" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="7">
         <v>251</v>
       </c>
-      <c r="B253" s="55" t="s">
-        <v>177</v>
+      <c r="B253" s="52" t="s">
+        <v>184</v>
       </c>
       <c r="C253" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D253" s="53" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="7">
         <v>252</v>
       </c>
-      <c r="B254" s="52" t="s">
+      <c r="B254" s="55" t="s">
         <v>184</v>
       </c>
       <c r="C254" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D254" s="53" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -7324,21 +7255,21 @@
         <v>9</v>
       </c>
       <c r="D255" s="53" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="7">
         <v>254</v>
       </c>
-      <c r="B256" s="55" t="s">
-        <v>184</v>
+      <c r="B256" s="52" t="s">
+        <v>188</v>
       </c>
       <c r="C256" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D256" s="53" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -7352,7 +7283,7 @@
         <v>9</v>
       </c>
       <c r="D257" s="53" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -7366,7 +7297,7 @@
         <v>9</v>
       </c>
       <c r="D258" s="53" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -7380,7 +7311,7 @@
         <v>9</v>
       </c>
       <c r="D259" s="53" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -7388,13 +7319,13 @@
         <v>258</v>
       </c>
       <c r="B260" s="52" t="s">
-        <v>188</v>
+        <v>321</v>
       </c>
       <c r="C260" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D260" s="53" t="s">
-        <v>328</v>
+        <v>717</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -7408,7 +7339,7 @@
         <v>9</v>
       </c>
       <c r="D261" s="53" t="s">
-        <v>717</v>
+        <v>723</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -7422,24 +7353,24 @@
         <v>9</v>
       </c>
       <c r="D262" s="53" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A263" s="7">
         <v>261</v>
       </c>
       <c r="B263" s="52" t="s">
-        <v>321</v>
+        <v>658</v>
       </c>
       <c r="C263" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D263" s="53" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="264" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="7">
         <v>262</v>
       </c>
@@ -7450,24 +7381,24 @@
         <v>9</v>
       </c>
       <c r="D264" s="53" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A265" s="7">
         <v>263</v>
       </c>
       <c r="B265" s="52" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C265" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D265" s="53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="266" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="7">
         <v>264</v>
       </c>
@@ -7478,24 +7409,24 @@
         <v>9</v>
       </c>
       <c r="D266" s="53" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A267" s="7">
         <v>265</v>
       </c>
       <c r="B267" s="52" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="C267" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D267" s="53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="268" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="7">
         <v>266</v>
       </c>
@@ -7506,24 +7437,24 @@
         <v>9</v>
       </c>
       <c r="D268" s="53" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A269" s="7">
         <v>267</v>
       </c>
       <c r="B269" s="52" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C269" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D269" s="53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="270" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="7">
         <v>268</v>
       </c>
@@ -7534,35 +7465,35 @@
         <v>9</v>
       </c>
       <c r="D270" s="53" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A271" s="7">
         <v>269</v>
       </c>
       <c r="B271" s="52" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C271" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D271" s="53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="272" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="7">
         <v>270</v>
       </c>
       <c r="B272" s="52" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C272" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D272" s="53" t="s">
-        <v>722</v>
+        <v>6</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -7570,13 +7501,13 @@
         <v>271</v>
       </c>
       <c r="B273" s="52" t="s">
-        <v>661</v>
+        <v>675</v>
       </c>
       <c r="C273" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D273" s="53" t="s">
-        <v>6</v>
+        <v>676</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -7590,7 +7521,7 @@
         <v>9</v>
       </c>
       <c r="D274" s="53" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -7604,7 +7535,7 @@
         <v>9</v>
       </c>
       <c r="D275" s="53" t="s">
-        <v>677</v>
+        <v>6</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
@@ -7612,13 +7543,13 @@
         <v>274</v>
       </c>
       <c r="B276" s="52" t="s">
-        <v>675</v>
+        <v>723</v>
       </c>
       <c r="C276" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D276" s="53" t="s">
-        <v>6</v>
+        <v>732</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
@@ -7626,26 +7557,12 @@
         <v>275</v>
       </c>
       <c r="B277" s="52" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C277" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D277" s="53" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A278" s="7">
-        <v>276</v>
-      </c>
-      <c r="B278" s="52" t="s">
-        <v>724</v>
-      </c>
-      <c r="C278" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D278" s="53" t="s">
         <v>733</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited <mathexpr> and <condexpr>
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlou\Documents\CompilerDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62154DB4-9790-4B25-823C-88AECCFD3C37}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33472A91-6A1B-4E58-A553-9BDF688966AE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
     <workbookView xWindow="-30" yWindow="7050" windowWidth="14400" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF02000000}"/>
@@ -21,7 +21,7 @@
     <sheet name="PREDICT TABLE" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">CFG!$A$1:$D$249</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">CFG!$A$1:$D$253</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'FOLLOW SET'!$A$1:$D$100</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3353" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3365" uniqueCount="901">
   <si>
     <t>#</t>
   </si>
@@ -2733,6 +2733,24 @@
   </si>
   <si>
     <t>INTERLUDE MUTE id(&lt;funcparam&gt;){ &lt;localdec&gt; &lt;statements&gt; }</t>
+  </si>
+  <si>
+    <t>&lt;nextmathexpr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;nextcondexpr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mathexpr&gt; &lt;nextmathexpr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;condexpr&gt; &lt;nextcondexpr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mathop&gt; &lt;mathexpr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;condop&gt; &lt;condexpr&gt;</t>
   </si>
 </sst>
 </file>
@@ -3657,13 +3675,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G277"/>
+  <dimension ref="A1:G281"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="1">
+      <selection activeCell="D248" sqref="D248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3674,7 +3692,7 @@
     <col min="4" max="4" width="53" style="56" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="55" customWidth="1"/>
     <col min="6" max="6" width="5.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="45.5703125" style="4" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -6824,7 +6842,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="7">
         <v>223</v>
       </c>
@@ -6838,7 +6856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="7">
         <v>224</v>
       </c>
@@ -6852,7 +6870,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="7">
         <v>225</v>
       </c>
@@ -6866,7 +6884,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="7">
         <v>226</v>
       </c>
@@ -6880,7 +6898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="7">
         <v>227</v>
       </c>
@@ -6891,10 +6909,13 @@
         <v>9</v>
       </c>
       <c r="D229" s="53" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+        <v>897</v>
+      </c>
+      <c r="E229" s="52"/>
+      <c r="F229" s="52"/>
+      <c r="G229" s="53"/>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="7">
         <v>228</v>
       </c>
@@ -6907,8 +6928,9 @@
       <c r="D230" s="53" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F230" s="52"/>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="7">
         <v>229</v>
       </c>
@@ -6921,8 +6943,10 @@
       <c r="D231" s="53" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F231" s="52"/>
+      <c r="G231" s="53"/>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="7">
         <v>230</v>
       </c>
@@ -6935,8 +6959,9 @@
       <c r="D232" s="53" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F232" s="52"/>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="7">
         <v>231</v>
       </c>
@@ -6949,8 +6974,9 @@
       <c r="D233" s="53" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F233" s="52"/>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="7">
         <v>232</v>
       </c>
@@ -6963,36 +6989,39 @@
       <c r="D234" s="53" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F234" s="52"/>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="7">
         <v>233</v>
       </c>
-      <c r="B235" s="52" t="s">
-        <v>167</v>
+      <c r="B235" s="55" t="s">
+        <v>895</v>
       </c>
       <c r="C235" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D235" s="53" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D235" s="4" t="s">
+        <v>899</v>
+      </c>
+      <c r="F235" s="52"/>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="7">
         <v>234</v>
       </c>
-      <c r="B236" s="52" t="s">
-        <v>167</v>
+      <c r="B236" s="55" t="s">
+        <v>895</v>
       </c>
       <c r="C236" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D236" s="53" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F236" s="52"/>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="7">
         <v>235</v>
       </c>
@@ -7003,10 +7032,10 @@
         <v>9</v>
       </c>
       <c r="D237" s="53" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="7">
         <v>236</v>
       </c>
@@ -7017,10 +7046,10 @@
         <v>9</v>
       </c>
       <c r="D238" s="53" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="7">
         <v>237</v>
       </c>
@@ -7031,21 +7060,21 @@
         <v>9</v>
       </c>
       <c r="D239" s="53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="7">
         <v>238</v>
       </c>
       <c r="B240" s="52" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C240" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D240" s="53" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -7053,13 +7082,13 @@
         <v>239</v>
       </c>
       <c r="B241" s="52" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C241" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D241" s="53" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -7073,7 +7102,7 @@
         <v>9</v>
       </c>
       <c r="D242" s="53" t="s">
-        <v>113</v>
+        <v>898</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -7087,7 +7116,7 @@
         <v>9</v>
       </c>
       <c r="D243" s="53" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7101,7 +7130,7 @@
         <v>9</v>
       </c>
       <c r="D244" s="53" t="s">
-        <v>321</v>
+        <v>113</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -7109,13 +7138,13 @@
         <v>243</v>
       </c>
       <c r="B245" s="52" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C245" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D245" s="53" t="s">
-        <v>177</v>
+        <v>116</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -7123,74 +7152,70 @@
         <v>244</v>
       </c>
       <c r="B246" s="52" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C246" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D246" s="53" t="s">
-        <v>184</v>
+        <v>321</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247" s="7">
-        <v>245</v>
-      </c>
-      <c r="B247" s="55" t="s">
-        <v>177</v>
+      <c r="A247" s="7"/>
+      <c r="B247" s="52" t="s">
+        <v>896</v>
       </c>
       <c r="C247" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D247" s="53" t="s">
-        <v>178</v>
+        <v>900</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="7">
-        <v>246</v>
-      </c>
-      <c r="B248" s="55" t="s">
-        <v>177</v>
+      <c r="A248" s="7"/>
+      <c r="B248" s="52" t="s">
+        <v>896</v>
       </c>
       <c r="C248" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D248" s="53" t="s">
-        <v>179</v>
+        <v>6</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="7">
-        <v>247</v>
-      </c>
-      <c r="B249" s="55" t="s">
+        <v>245</v>
+      </c>
+      <c r="B249" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="C249" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D249" s="53" t="s">
         <v>177</v>
-      </c>
-      <c r="C249" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D249" s="53" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="7">
-        <v>248</v>
-      </c>
-      <c r="B250" s="55" t="s">
-        <v>177</v>
+        <v>246</v>
+      </c>
+      <c r="B250" s="52" t="s">
+        <v>176</v>
       </c>
       <c r="C250" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D250" s="53" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="7">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B251" s="55" t="s">
         <v>177</v>
@@ -7199,12 +7224,12 @@
         <v>9</v>
       </c>
       <c r="D251" s="53" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="7">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B252" s="55" t="s">
         <v>177</v>
@@ -7213,225 +7238,225 @@
         <v>9</v>
       </c>
       <c r="D252" s="53" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="7">
-        <v>251</v>
-      </c>
-      <c r="B253" s="52" t="s">
-        <v>184</v>
+        <v>249</v>
+      </c>
+      <c r="B253" s="55" t="s">
+        <v>177</v>
       </c>
       <c r="C253" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D253" s="53" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="7">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B254" s="55" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C254" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D254" s="53" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="7">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B255" s="55" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C255" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D255" s="53" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="7">
-        <v>254</v>
-      </c>
-      <c r="B256" s="52" t="s">
-        <v>188</v>
+        <v>252</v>
+      </c>
+      <c r="B256" s="55" t="s">
+        <v>177</v>
       </c>
       <c r="C256" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D256" s="53" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="7">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B257" s="52" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C257" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D257" s="53" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="7">
-        <v>256</v>
-      </c>
-      <c r="B258" s="52" t="s">
-        <v>188</v>
+        <v>254</v>
+      </c>
+      <c r="B258" s="55" t="s">
+        <v>184</v>
       </c>
       <c r="C258" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D258" s="53" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="7">
-        <v>257</v>
-      </c>
-      <c r="B259" s="52" t="s">
-        <v>188</v>
+        <v>255</v>
+      </c>
+      <c r="B259" s="55" t="s">
+        <v>184</v>
       </c>
       <c r="C259" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D259" s="53" t="s">
-        <v>328</v>
+        <v>187</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="7">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B260" s="52" t="s">
-        <v>321</v>
+        <v>188</v>
       </c>
       <c r="C260" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D260" s="53" t="s">
-        <v>717</v>
+        <v>189</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="7">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B261" s="52" t="s">
-        <v>321</v>
+        <v>188</v>
       </c>
       <c r="C261" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D261" s="53" t="s">
-        <v>723</v>
+        <v>190</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="7">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B262" s="52" t="s">
-        <v>321</v>
+        <v>188</v>
       </c>
       <c r="C262" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D262" s="53" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="263" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="7">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B263" s="52" t="s">
-        <v>658</v>
+        <v>188</v>
       </c>
       <c r="C263" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D263" s="53" t="s">
-        <v>718</v>
+        <v>328</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="7">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B264" s="52" t="s">
-        <v>658</v>
+        <v>321</v>
       </c>
       <c r="C264" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D264" s="53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="7">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B265" s="52" t="s">
-        <v>659</v>
+        <v>321</v>
       </c>
       <c r="C265" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D265" s="53" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="7">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B266" s="52" t="s">
-        <v>659</v>
+        <v>321</v>
       </c>
       <c r="C266" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D266" s="53" t="s">
-        <v>6</v>
+        <v>724</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A267" s="7">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B267" s="52" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C267" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D267" s="53" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="7">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B268" s="52" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C268" s="52" t="s">
         <v>9</v>
@@ -7442,24 +7467,24 @@
     </row>
     <row r="269" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A269" s="7">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B269" s="52" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C269" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D269" s="53" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="7">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B270" s="52" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C270" s="52" t="s">
         <v>9</v>
@@ -7470,24 +7495,24 @@
     </row>
     <row r="271" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A271" s="7">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B271" s="52" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C271" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D271" s="53" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="7">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B272" s="52" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C272" s="52" t="s">
         <v>9</v>
@@ -7496,73 +7521,129 @@
         <v>6</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A273" s="7">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B273" s="52" t="s">
-        <v>675</v>
+        <v>661</v>
       </c>
       <c r="C273" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D273" s="53" t="s">
-        <v>676</v>
+        <v>721</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" s="7">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B274" s="52" t="s">
-        <v>675</v>
+        <v>661</v>
       </c>
       <c r="C274" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D274" s="53" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A275" s="7">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B275" s="52" t="s">
-        <v>675</v>
+        <v>662</v>
       </c>
       <c r="C275" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D275" s="53" t="s">
-        <v>6</v>
+        <v>722</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="7">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B276" s="52" t="s">
-        <v>723</v>
+        <v>661</v>
       </c>
       <c r="C276" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D276" s="53" t="s">
-        <v>732</v>
+        <v>6</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="7">
+        <v>273</v>
+      </c>
+      <c r="B277" s="52" t="s">
+        <v>675</v>
+      </c>
+      <c r="C277" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D277" s="53" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="7">
+        <v>274</v>
+      </c>
+      <c r="B278" s="52" t="s">
+        <v>675</v>
+      </c>
+      <c r="C278" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D278" s="53" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="7">
         <v>275</v>
       </c>
-      <c r="B277" s="52" t="s">
+      <c r="B279" s="52" t="s">
+        <v>675</v>
+      </c>
+      <c r="C279" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D279" s="53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="7">
+        <v>276</v>
+      </c>
+      <c r="B280" s="52" t="s">
+        <v>723</v>
+      </c>
+      <c r="C280" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D280" s="53" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" s="7">
+        <v>277</v>
+      </c>
+      <c r="B281" s="52" t="s">
         <v>724</v>
       </c>
-      <c r="C277" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D277" s="53" t="s">
+      <c r="C281" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D281" s="53" t="s">
         <v>733</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added identifiers as array value
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marlou\Documents\CompilerDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588CC718-0D79-41EC-A1A3-15B37C32DC39}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7691EF30-F3DF-41F6-9A31-5AE0E8C0E824}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
     <workbookView xWindow="-30" yWindow="7050" windowWidth="14400" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF02000000}"/>
@@ -2597,9 +2597,6 @@
     <t>&lt;2dintarrval&gt;</t>
   </si>
   <si>
-    <t>INT_LIT &lt;next1dintarrval&gt;</t>
-  </si>
-  <si>
     <t>&lt;next1dintarrval&gt;</t>
   </si>
   <si>
@@ -2642,9 +2639,6 @@
     <t>, &lt;2dfloatarrval&gt;</t>
   </si>
   <si>
-    <t>FLOAT_LIT &lt;next1dfloatarrval&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> = { &lt;chararrval&gt; }</t>
   </si>
   <si>
@@ -2669,9 +2663,6 @@
     <t>, &lt;2dchararrval&gt;</t>
   </si>
   <si>
-    <t>CHAR_LIT &lt;next1dchararrval&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> = { &lt;strarrval&gt; }</t>
   </si>
   <si>
@@ -2696,9 +2687,6 @@
     <t>, &lt;2dstrarrval&gt;</t>
   </si>
   <si>
-    <t>STRING_LIT &lt;next1dstrarrval&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> = { &lt;boolarrval&gt; }</t>
   </si>
   <si>
@@ -2723,9 +2711,6 @@
     <t>, &lt;2dboolarrval&gt;</t>
   </si>
   <si>
-    <t>BOOL_LIT &lt;next1dboolarrval&gt;</t>
-  </si>
-  <si>
     <t>PRELUDE &lt;global&gt; CONCERT(){ &lt;localdec&gt; &lt;statements&gt; } ENCORE</t>
   </si>
   <si>
@@ -2751,6 +2736,21 @@
   </si>
   <si>
     <t>&lt;condop&gt; &lt;condexpr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;intval&gt; &lt;next1dintarrval&gt;</t>
+  </si>
+  <si>
+    <t>&lt;charval&gt; &lt;next1dchararrval&gt;</t>
+  </si>
+  <si>
+    <t>&lt;floatval&gt; &lt;next1dfloatarrval&gt;</t>
+  </si>
+  <si>
+    <t>&lt;strval&gt; &lt;next1dstrarrval&gt;</t>
+  </si>
+  <si>
+    <t>&lt;boolval&gt; &lt;next1dboolarrval&gt;</t>
   </si>
 </sst>
 </file>
@@ -3420,7 +3420,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3472,7 +3472,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3680,8 +3680,8 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="1">
-      <selection activeCell="D283" sqref="D283"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="1">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3690,7 +3690,7 @@
     <col min="2" max="2" width="23.140625" style="48" customWidth="1"/>
     <col min="3" max="3" width="5.140625" style="48" customWidth="1"/>
     <col min="4" max="4" width="53" style="56" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" style="55" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" style="55" customWidth="1"/>
     <col min="6" max="6" width="5.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="45.5703125" style="4" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="4"/>
@@ -3730,7 +3730,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4892,7 +4892,7 @@
         <v>9</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F86" s="52"/>
     </row>
@@ -4954,7 +4954,7 @@
         <v>9</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>849</v>
+        <v>896</v>
       </c>
       <c r="F90" s="52"/>
     </row>
@@ -4963,13 +4963,13 @@
         <v>89</v>
       </c>
       <c r="B91" s="55" t="s">
+        <v>849</v>
+      </c>
+      <c r="C91" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>850</v>
-      </c>
-      <c r="C91" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>851</v>
       </c>
       <c r="F91" s="52"/>
     </row>
@@ -4978,7 +4978,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="55" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C92" s="52" t="s">
         <v>9</v>
@@ -5000,7 +5000,7 @@
         <v>9</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F93" s="52"/>
     </row>
@@ -5009,13 +5009,13 @@
         <v>92</v>
       </c>
       <c r="B94" s="55" t="s">
+        <v>852</v>
+      </c>
+      <c r="C94" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" s="4" t="s">
         <v>853</v>
-      </c>
-      <c r="C94" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>854</v>
       </c>
       <c r="F94" s="52"/>
     </row>
@@ -5024,7 +5024,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="55" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C95" s="52" t="s">
         <v>9</v>
@@ -5046,7 +5046,7 @@
         <v>9</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F96" s="52"/>
     </row>
@@ -5075,7 +5075,7 @@
         <v>9</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -5089,7 +5089,7 @@
         <v>9</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -5097,13 +5097,13 @@
         <v>98</v>
       </c>
       <c r="B100" s="55" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C100" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>864</v>
+        <v>898</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -5111,13 +5111,13 @@
         <v>99</v>
       </c>
       <c r="B101" s="55" t="s">
+        <v>858</v>
+      </c>
+      <c r="C101" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" s="4" t="s">
         <v>859</v>
-      </c>
-      <c r="C101" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -5125,7 +5125,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="55" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C102" s="52" t="s">
         <v>9</v>
@@ -5139,13 +5139,13 @@
         <v>101</v>
       </c>
       <c r="B103" s="55" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C103" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -5153,13 +5153,13 @@
         <v>102</v>
       </c>
       <c r="B104" s="55" t="s">
+        <v>861</v>
+      </c>
+      <c r="C104" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" s="4" t="s">
         <v>862</v>
-      </c>
-      <c r="C104" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -5167,7 +5167,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="55" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C105" s="52" t="s">
         <v>9</v>
@@ -5187,7 +5187,7 @@
         <v>9</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -5215,7 +5215,7 @@
         <v>9</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -5229,7 +5229,7 @@
         <v>9</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -5237,13 +5237,13 @@
         <v>108</v>
       </c>
       <c r="B110" s="55" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="C110" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>873</v>
+        <v>897</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -5251,13 +5251,13 @@
         <v>109</v>
       </c>
       <c r="B111" s="55" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C111" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -5265,7 +5265,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="55" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C112" s="52" t="s">
         <v>9</v>
@@ -5279,13 +5279,13 @@
         <v>111</v>
       </c>
       <c r="B113" s="55" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C113" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -5293,13 +5293,13 @@
         <v>112</v>
       </c>
       <c r="B114" s="55" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C114" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -5307,7 +5307,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="55" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C115" s="52" t="s">
         <v>9</v>
@@ -5327,7 +5327,7 @@
         <v>9</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -5355,7 +5355,7 @@
         <v>9</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5369,7 +5369,7 @@
         <v>9</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -5377,13 +5377,13 @@
         <v>118</v>
       </c>
       <c r="B120" s="55" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="C120" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>882</v>
+        <v>899</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -5391,13 +5391,13 @@
         <v>119</v>
       </c>
       <c r="B121" s="55" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="C121" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -5405,7 +5405,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="55" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="C122" s="52" t="s">
         <v>9</v>
@@ -5419,13 +5419,13 @@
         <v>121</v>
       </c>
       <c r="B123" s="55" t="s">
+        <v>873</v>
+      </c>
+      <c r="C123" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" s="4" t="s">
         <v>876</v>
-      </c>
-      <c r="C123" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D123" s="4" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -5433,13 +5433,13 @@
         <v>122</v>
       </c>
       <c r="B124" s="55" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="C124" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -5447,7 +5447,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="55" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="C125" s="52" t="s">
         <v>9</v>
@@ -5467,7 +5467,7 @@
         <v>9</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -5495,7 +5495,7 @@
         <v>9</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5509,7 +5509,7 @@
         <v>9</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -5517,13 +5517,13 @@
         <v>128</v>
       </c>
       <c r="B130" s="55" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="C130" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>891</v>
+        <v>900</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -5531,13 +5531,13 @@
         <v>129</v>
       </c>
       <c r="B131" s="55" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C131" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5545,7 +5545,7 @@
         <v>130</v>
       </c>
       <c r="B132" s="55" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C132" s="52" t="s">
         <v>9</v>
@@ -5559,13 +5559,13 @@
         <v>131</v>
       </c>
       <c r="B133" s="55" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="C133" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -5573,13 +5573,13 @@
         <v>132</v>
       </c>
       <c r="B134" s="55" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="C134" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -5587,7 +5587,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="55" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="C135" s="52" t="s">
         <v>9</v>
@@ -5607,7 +5607,7 @@
         <v>9</v>
       </c>
       <c r="D136" s="53" t="s">
-        <v>893</v>
+        <v>888</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -5621,7 +5621,7 @@
         <v>9</v>
       </c>
       <c r="D137" s="53" t="s">
-        <v>894</v>
+        <v>889</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -6909,7 +6909,7 @@
         <v>9</v>
       </c>
       <c r="D229" s="53" t="s">
-        <v>897</v>
+        <v>892</v>
       </c>
       <c r="E229" s="52"/>
       <c r="F229" s="52"/>
@@ -6996,13 +6996,13 @@
         <v>233</v>
       </c>
       <c r="B235" s="55" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="C235" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D235" s="4" t="s">
-        <v>899</v>
+        <v>894</v>
       </c>
       <c r="F235" s="52"/>
     </row>
@@ -7011,7 +7011,7 @@
         <v>234</v>
       </c>
       <c r="B236" s="55" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="C236" s="52" t="s">
         <v>9</v>
@@ -7102,7 +7102,7 @@
         <v>9</v>
       </c>
       <c r="D242" s="53" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -7166,13 +7166,13 @@
         <v>245</v>
       </c>
       <c r="B247" s="52" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
       <c r="C247" s="52" t="s">
         <v>9</v>
       </c>
       <c r="D247" s="53" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -7180,7 +7180,7 @@
         <v>246</v>
       </c>
       <c r="B248" s="52" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
       <c r="C248" s="52" t="s">
         <v>9</v>

</xml_diff>